<commit_message>
implementing database testing and UI testing is started
</commit_message>
<xml_diff>
--- a/Data/myData.xlsx
+++ b/Data/myData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>clinet name</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>//div[contains(@class,'alert')]</t>
+  </si>
+  <si>
+    <t>Gandhali16</t>
   </si>
 </sst>
 </file>
@@ -691,11 +694,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
@@ -755,7 +761,7 @@
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1">
       <c r="A2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>

</xml_diff>